<commit_message>
changed test case language to EN
</commit_message>
<xml_diff>
--- a/website/databaza_dopravcov.xlsx
+++ b/website/databaza_dopravcov.xlsx
@@ -569,15 +569,15 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +1003,7 @@
         <v>95</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>